<commit_message>
readjusted for correct loading of packages
</commit_message>
<xml_diff>
--- a/WGUPS Package File.xlsx
+++ b/WGUPS Package File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miguel.dehoyos\Downloads\C950\New Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redre\Desktop\WGU\C950\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7D6FC3F-E74F-4587-BEDF-A00C8FAE7100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DC0C8D-F0CB-4875-8458-26A23C956652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,12 +222,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -257,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -269,7 +293,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -280,12 +303,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -298,6 +315,28 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,7 +365,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>929640</xdr:colOff>
+      <xdr:colOff>843915</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>115169</xdr:rowOff>
     </xdr:to>
@@ -635,1101 +674,1103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H6"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" customWidth="1"/>
-    <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="39.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+    <row r="1" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+    <row r="2" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+    <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+    <row r="5" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+    <row r="9" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>1</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="C9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="12">
         <v>84115</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="12">
         <v>21</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
         <v>2</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="C10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="15">
         <v>84106</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="9">
+      <c r="F10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="15">
         <v>44</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <v>3</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="C11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="15">
         <v>84103</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="9">
+      <c r="F11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="15">
         <v>2</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+    <row r="12" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>4</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="C12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="12">
         <v>84115</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="F12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="12">
         <v>4</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="H12" s="13"/>
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>5</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="9">
+      <c r="C13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12">
         <v>84111</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="9">
+      <c r="F13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="12">
         <v>5</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
-        <v>6</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="H13" s="13"/>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>6</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="9">
+      <c r="D14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="15">
         <v>84119</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="17">
         <v>0.4375</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="15">
         <v>88</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="15">
         <v>84106</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="F15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="15">
         <v>8</v>
       </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
         <v>8</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="9">
+      <c r="C16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="15">
         <v>84103</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="9">
-        <v>9</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="F16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="15">
+        <v>9</v>
+      </c>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>9</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="C17" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="18">
         <v>84103</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="9">
+      <c r="F17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="18">
         <v>2</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+    <row r="18" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
         <v>10</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="9">
+      <c r="C18" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="15">
         <v>84105</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="9">
+      <c r="F18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="15">
         <v>1</v>
       </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
         <v>11</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="9">
+      <c r="C19" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="15">
         <v>84118</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="9">
+      <c r="F19" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="15">
         <v>1</v>
       </c>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
         <v>12</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="9">
+      <c r="D20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="15">
         <v>84119</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="9">
+      <c r="F20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="15">
         <v>1</v>
       </c>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
         <v>13</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="9">
+      <c r="C21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="12">
         <v>84104</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="12">
         <v>2</v>
       </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
         <v>14</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="9">
+      <c r="D22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="12">
         <v>84117</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="12">
         <v>88</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+    <row r="23" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
         <v>15</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="9">
+      <c r="D23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="12">
         <v>84117</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="14">
         <v>0.375</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="12">
         <v>4</v>
       </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
         <v>16</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="9">
+      <c r="D24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="12">
         <v>84117</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="12">
         <v>88</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
+    <row r="25" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
         <v>17</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="9">
+      <c r="C25" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="18">
         <v>84119</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="9">
+      <c r="F25" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="18">
         <v>2</v>
       </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
         <v>18</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="9">
+      <c r="C26" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="15">
         <v>84123</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="9">
-        <v>6</v>
-      </c>
-      <c r="H26" s="4" t="s">
+      <c r="F26" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="15">
+        <v>6</v>
+      </c>
+      <c r="H26" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
+    <row r="27" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
         <v>19</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="9">
+      <c r="C27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="12">
         <v>84115</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="9">
+      <c r="F27" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="12">
         <v>37</v>
       </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
         <v>20</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="9">
+      <c r="C28" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="12">
         <v>84115</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="12">
         <v>37</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+    <row r="29" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
         <v>21</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="9">
+      <c r="C29" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="18">
         <v>84115</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="9">
+      <c r="F29" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="18">
         <v>3</v>
       </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
+      <c r="H29" s="19"/>
+    </row>
+    <row r="30" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
         <v>22</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="9">
+      <c r="D30" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="18">
         <v>84121</v>
       </c>
-      <c r="F30" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="9">
+      <c r="F30" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="18">
         <v>2</v>
       </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
+      <c r="H30" s="19"/>
+    </row>
+    <row r="31" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
         <v>23</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="9">
+      <c r="C31" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="18">
         <v>84118</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="9">
+      <c r="F31" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="18">
         <v>5</v>
       </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
         <v>24</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="9">
+      <c r="D32" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="18">
         <v>84107</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="9">
-        <v>7</v>
-      </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
+      <c r="F32" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="18">
+        <v>7</v>
+      </c>
+      <c r="H32" s="19"/>
+    </row>
+    <row r="33" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
         <v>25</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="9">
+      <c r="C33" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="15">
         <v>84117</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="17">
         <v>0.4375</v>
       </c>
-      <c r="G33" s="9">
-        <v>7</v>
-      </c>
-      <c r="H33" s="4" t="s">
+      <c r="G33" s="15">
+        <v>7</v>
+      </c>
+      <c r="H33" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
+    <row r="34" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="18">
         <v>26</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="9">
+      <c r="C34" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="18">
         <v>84117</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="9">
+      <c r="F34" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="18">
         <v>25</v>
       </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9">
+      <c r="H34" s="19"/>
+    </row>
+    <row r="35" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
         <v>27</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="9">
+      <c r="C35" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="18">
         <v>84104</v>
       </c>
-      <c r="F35" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="F35" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="18">
         <v>5</v>
       </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9">
+      <c r="H35" s="19"/>
+    </row>
+    <row r="36" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
         <v>28</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="9">
+      <c r="C36" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="15">
         <v>84115</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="9">
-        <v>7</v>
-      </c>
-      <c r="H36" s="4" t="s">
+      <c r="F36" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="15">
+        <v>7</v>
+      </c>
+      <c r="H36" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9">
+    <row r="37" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
         <v>29</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="9">
+      <c r="C37" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="12">
         <v>84106</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="12">
         <v>2</v>
       </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9">
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>30</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="9">
+      <c r="C38" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="12">
         <v>84103</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="12">
         <v>1</v>
       </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
         <v>31</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="9">
+      <c r="C39" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="12">
         <v>84119</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F39" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="12">
         <v>1</v>
       </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9">
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
         <v>32</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="9">
+      <c r="C40" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="15">
         <v>84119</v>
       </c>
-      <c r="F40" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="9">
+      <c r="F40" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="15">
         <v>1</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="9">
+    <row r="41" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18">
         <v>33</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="9">
+      <c r="C41" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="18">
         <v>84106</v>
       </c>
-      <c r="F41" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="9">
+      <c r="F41" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="18">
         <v>1</v>
       </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9">
+      <c r="H41" s="19"/>
+    </row>
+    <row r="42" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
         <v>34</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="9">
+      <c r="D42" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="12">
         <v>84117</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F42" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="12">
         <v>2</v>
       </c>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9">
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18">
         <v>35</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="9">
+      <c r="C43" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="18">
         <v>84104</v>
       </c>
-      <c r="F43" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="9">
+      <c r="F43" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="18">
         <v>88</v>
       </c>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="9">
+      <c r="H43" s="19"/>
+    </row>
+    <row r="44" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
         <v>36</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="9">
+      <c r="D44" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="15">
         <v>84119</v>
       </c>
-      <c r="F44" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G44" s="9">
+      <c r="F44" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="15">
         <v>88</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="H44" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9">
+    <row r="45" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
         <v>37</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="9">
+      <c r="C45" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="12">
         <v>84111</v>
       </c>
-      <c r="F45" s="10">
+      <c r="F45" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="12">
         <v>2</v>
       </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9">
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
         <v>38</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="9">
+      <c r="C46" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="15">
         <v>84111</v>
       </c>
-      <c r="F46" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="9">
-        <v>9</v>
-      </c>
-      <c r="H46" s="4" t="s">
+      <c r="F46" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="15">
+        <v>9</v>
+      </c>
+      <c r="H46" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="9">
+    <row r="47" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18">
         <v>39</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="9">
+      <c r="C47" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="18">
         <v>84104</v>
       </c>
-      <c r="F47" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="9">
-        <v>9</v>
-      </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="9">
+      <c r="F47" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="18">
+        <v>9</v>
+      </c>
+      <c r="H47" s="19"/>
+    </row>
+    <row r="48" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
         <v>40</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="9">
+      <c r="C48" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="12">
         <v>84115</v>
       </c>
-      <c r="F48" s="10">
+      <c r="F48" s="14">
         <v>0.4375</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="12">
         <v>45</v>
       </c>
-      <c r="H48" s="4"/>
+      <c r="H48" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1753,55 +1794,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Step_x0020_Completed>
-    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Editor0>
-    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Performance_x0020_Steps_x0020_Completed>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Specifications xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Clone xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <AssessmentType xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <AssessmentCode xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <PDO xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </PDO>
-    <TaxCatchAll xmlns="1f707338-ea0f-4fe5-baee-59b996692b22" xsi:nil="true"/>
-    <_x0033_rdPartyCertVendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2311,6 +2303,55 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Step_x0020_Completed>
+    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Editor0>
+    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Performance_x0020_Steps_x0020_Completed>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Specifications xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Clone xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <AssessmentType xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <AssessmentCode xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <PDO xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </PDO>
+    <TaxCatchAll xmlns="1f707338-ea0f-4fe5-baee-59b996692b22" xsi:nil="true"/>
+    <_x0033_rdPartyCertVendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
   <ds:schemaRefs>
@@ -2320,6 +2361,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5214019-7508-47A8-9FC8-EDBE31C095C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC0CE6-074E-44A2-B54E-38496285A228}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2333,10 +2394,7 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5214019-7508-47A8-9FC8-EDBE31C095C4}"/>
 </file>
</xml_diff>